<commit_message>
updated Salary, added Bonus Dates & Benefits
</commit_message>
<xml_diff>
--- a/VISBAL-BUDGET.xlsx
+++ b/VISBAL-BUDGET.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27204"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/51a4521e86238ef2/Documents/Personal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="208" documentId="13_ncr:1_{CBFD40BC-3771-4577-82BB-E96CB70EFBB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FEA9BB9-27CD-49D8-A695-5AF0F4FB0885}"/>
+  <xr:revisionPtr revIDLastSave="299" documentId="13_ncr:1_{CBFD40BC-3771-4577-82BB-E96CB70EFBB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F89F1D7-3CEC-408B-9119-6494FC27C0F1}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-9315" windowWidth="38640" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NOTES" sheetId="2" r:id="rId1"/>
@@ -34,8 +34,115 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Alex Visbal</author>
+  </authors>
+  <commentList>
+    <comment ref="H13" authorId="0" shapeId="0" xr:uid="{058EE677-2EA5-43F4-AB70-D03022DE28A0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alex Visbal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+March 15th [Per Kerry's Offer Letter]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H14" authorId="0" shapeId="0" xr:uid="{AA5AC5EE-E1B8-4187-80E5-0E3F27597042}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alex Visbal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Guessing June 15th? [Per the Pattern]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H15" authorId="0" shapeId="0" xr:uid="{D6272EA6-7878-4CFA-8B07-CCB7C24B4F10}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Alex Visbal:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+September 15th [Per Kerry's Offer Letter]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H16" authorId="0" shapeId="0" xr:uid="{AC9803E0-D899-42D1-8723-3164B22CC494}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alex Visbal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Dec 29th [2023 Bonus Date]</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
   <si>
     <t>Total monthly income</t>
   </si>
@@ -79,9 +186,6 @@
     <t>Savings</t>
   </si>
   <si>
-    <t>IRA &amp; Brokerage</t>
-  </si>
-  <si>
     <t>Automobile Gasoline</t>
   </si>
   <si>
@@ -103,9 +207,6 @@
     <t>Massage Envy Membership</t>
   </si>
   <si>
-    <t>Buffer</t>
-  </si>
-  <si>
     <t>Total Expected Bonuses =</t>
   </si>
   <si>
@@ -173,6 +274,41 @@
   </si>
   <si>
     <t>Roth 401k</t>
+  </si>
+  <si>
+    <t>IRA &amp; Traditional</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="14"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Actualize Benefits:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1. No Healthcare Coverage Cost
+2. 3% 401k Match
+3. $300/month HSA Contribution
+4. $750/year Wellness Bonus
+5. $2500/year Learning Bonus</t>
+    </r>
+  </si>
+  <si>
+    <t>C:\Users\avisb\OneDrive\Documents\Personal</t>
   </si>
 </sst>
 </file>
@@ -185,7 +321,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -303,15 +439,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <i/>
-      <sz val="12"/>
-      <color theme="1" tint="0.34998626667073579"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
@@ -360,8 +487,37 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -388,12 +544,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFEFFE7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -405,7 +555,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -524,19 +674,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -562,39 +699,6 @@
       <top style="thick">
         <color indexed="64"/>
       </top>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -607,91 +711,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -796,8 +815,47 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
       <right/>
       <top style="thin">
@@ -809,15 +867,170 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color theme="0"/>
       </right>
       <top style="thin">
         <color theme="0"/>
       </top>
-      <bottom style="thin">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
         <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -829,10 +1042,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -842,205 +1055,220 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="8" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="8" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="8" fontId="10" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="8" fontId="9" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="17" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="21" fillId="6" borderId="0" xfId="7" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="21" fillId="6" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="5" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="7" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="19" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="20" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="21" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="22" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="8" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="9" fillId="2" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="8" fillId="3" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="6" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="17" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="17" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="8" fontId="18" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="17" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="18" fillId="4" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="5" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="6" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="30" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="31" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="32" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="33" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="8" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="9" fillId="2" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="8" fillId="3" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="22" fillId="7" borderId="0" xfId="7" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="22" fillId="7" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="31" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="17" fillId="4" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Currency" xfId="7" builtinId="4"/>
@@ -1092,39 +1320,8 @@
       </font>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left/>
-        <right/>
-        <top style="thick">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thick">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1" tint="0.34998626667073579"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thick">
-          <color indexed="64"/>
-        </left>
         <right/>
         <top style="thick">
           <color indexed="64"/>
@@ -1154,6 +1351,37 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thick">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thick">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1487,7 +1715,7 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>732305</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>7750</xdr:rowOff>
+      <xdr:rowOff>17275</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1519,8 +1747,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="709146" y="387443"/>
-          <a:ext cx="679450" cy="696072"/>
+          <a:off x="745005" y="392486"/>
+          <a:ext cx="673100" cy="691589"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1537,14 +1765,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Housing" displayName="Housing" ref="C11:D23" totalsRowCount="1" headerRowDxfId="11" dataDxfId="9" totalsRowDxfId="7" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="6">
-  <autoFilter ref="C11:D22" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Housing" displayName="Housing" ref="C11:D22" totalsRowCount="1" headerRowDxfId="11" dataDxfId="9" totalsRowDxfId="7" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+  <autoFilter ref="C11:D21" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Category" totalsRowLabel="Subtotal" dataDxfId="5" totalsRowDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Cost" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Category" totalsRowLabel="Subtotal" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Cost" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="Address Book" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1764,208 +1992,210 @@
   <dimension ref="B2:K17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+      <selection activeCell="C9" sqref="B3:K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="11" width="8.09765625" customWidth="1"/>
+    <col min="3" max="11" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="38">
+    <row r="2" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B3" s="21">
         <v>1</v>
       </c>
-      <c r="C3" s="41" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="43"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="39"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="46"/>
-    </row>
-    <row r="5" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="40"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="49"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="38">
+      <c r="C3" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="26"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B4" s="22"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="29"/>
+    </row>
+    <row r="5" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="23"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="32"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B6" s="21">
         <v>2</v>
       </c>
-      <c r="C6" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="43"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="39"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="46"/>
-    </row>
-    <row r="8" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="40"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="49"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B9" s="38">
+      <c r="C6" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="26"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B7" s="22"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="29"/>
+    </row>
+    <row r="8" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="23"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="32"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B9" s="21">
         <v>3</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="42"/>
-      <c r="K9" s="43"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B10" s="39"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="45"/>
-      <c r="K10" s="46"/>
-    </row>
-    <row r="11" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="40"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="49"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="38">
+      <c r="C9" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="26"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B10" s="22"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="29"/>
+    </row>
+    <row r="11" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="23"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="32"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B12" s="21">
         <v>4</v>
       </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="43"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="39"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="45"/>
-      <c r="K13" s="46"/>
-    </row>
-    <row r="14" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="40"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="49"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="38">
+      <c r="C12" s="24"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="26"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B13" s="22"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="29"/>
+    </row>
+    <row r="14" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="23"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="32"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B15" s="21">
         <v>5</v>
       </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="42"/>
-      <c r="K15" s="43"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="39"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="45"/>
-      <c r="J16" s="45"/>
-      <c r="K16" s="46"/>
-    </row>
-    <row r="17" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="40"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="49"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="26"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B16" s="22"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="29"/>
+    </row>
+    <row r="17" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="23"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1983,432 +2213,464 @@
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{2297F6CE-DB87-4DC5-A4D7-E628DE96DED3}"/>
     <hyperlink ref="C6" r:id="rId2" location="/Myself/PayandAnnualStatements" xr:uid="{559C8455-670D-48EF-972B-36EEE7F143FF}"/>
+    <hyperlink ref="C9" r:id="rId3" xr:uid="{7C755A49-5F67-41F0-BCE7-F3E8AAAAD5C3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:O28"/>
+  <dimension ref="B2:O27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="30" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="30" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.8984375" customWidth="1"/>
-    <col min="2" max="2" width="1.3984375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="39.3984375" customWidth="1"/>
-    <col min="4" max="4" width="26.3984375" customWidth="1"/>
-    <col min="7" max="7" width="15.69921875" customWidth="1"/>
-    <col min="8" max="8" width="15.296875" style="33" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.796875" customWidth="1"/>
-    <col min="11" max="11" width="11.3984375" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="1.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" customWidth="1"/>
     <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" s="1" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:15" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3"/>
-      <c r="H2" s="32"/>
-    </row>
-    <row r="3" spans="2:15" s="1" customFormat="1" ht="52" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="2:15" s="1" customFormat="1" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5"/>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="54"/>
-    </row>
-    <row r="4" spans="2:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="73" t="s">
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
+    </row>
+    <row r="4" spans="2:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="74"/>
-      <c r="E4" s="57" t="s">
+      <c r="D4" s="63"/>
+      <c r="E4" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="59"/>
-      <c r="K4" s="77" t="s">
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="63"/>
+      <c r="K4" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" s="45"/>
+      <c r="N4" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="O4" s="45"/>
+    </row>
+    <row r="5" spans="2:15" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="69" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="7">
+        <v>4000</v>
+      </c>
+      <c r="E5" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="35"/>
+      <c r="G5" s="40">
+        <f>D8</f>
+        <v>8000</v>
+      </c>
+      <c r="H5" s="41"/>
+      <c r="I5" s="37"/>
+      <c r="K5" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" s="19">
+        <v>296</v>
+      </c>
+      <c r="N5" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" s="20">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="69" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="7">
+        <v>4000</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="37"/>
+      <c r="G6" s="42">
+        <f>Housing[[#Totals],[Cost]]</f>
+        <v>5779</v>
+      </c>
+      <c r="H6" s="41"/>
+      <c r="I6" s="37"/>
+      <c r="K6" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="L4" s="77"/>
-      <c r="N4" s="77" t="s">
+      <c r="L6" s="19">
+        <f>O8</f>
+        <v>240</v>
+      </c>
+      <c r="N6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="O6" s="46">
+        <f>D14-791</f>
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="69" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0</v>
+      </c>
+      <c r="E7" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="39"/>
+      <c r="G7" s="43">
+        <f>G5-G6</f>
+        <v>2221</v>
+      </c>
+      <c r="H7" s="44"/>
+      <c r="I7" s="39"/>
+      <c r="N7" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="O7" s="20">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="8">
+        <f>SUM(D5:D7)</f>
+        <v>8000</v>
+      </c>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="71"/>
+      <c r="N8" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="O8" s="20">
+        <f>(D5+D6)*0.03</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="72"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="71"/>
+      <c r="N9" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="O4" s="77"/>
-    </row>
-    <row r="5" spans="2:15" ht="24.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="9">
-        <v>3845</v>
-      </c>
-      <c r="E5" s="60" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="61"/>
-      <c r="G5" s="66">
-        <f>D8</f>
-        <v>7690</v>
-      </c>
-      <c r="H5" s="67"/>
-      <c r="I5" s="68"/>
-      <c r="K5" s="76" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" s="78">
-        <v>296</v>
-      </c>
-      <c r="N5" s="76" t="s">
-        <v>40</v>
-      </c>
-      <c r="O5" s="79">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="9">
-        <v>3845</v>
-      </c>
-      <c r="E6" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="63"/>
-      <c r="G6" s="69">
-        <f>Housing[[#Totals],[Cost]]</f>
-        <v>6238</v>
-      </c>
-      <c r="H6" s="67"/>
-      <c r="I6" s="68"/>
-      <c r="K6" s="76" t="s">
-        <v>41</v>
-      </c>
-      <c r="L6" s="78"/>
-      <c r="N6" s="76" t="s">
+      <c r="O9" s="20">
+        <f>SUM(O5:O8)</f>
+        <v>2836</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" s="2" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B10" s="6"/>
+      <c r="C10" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="33"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="74"/>
+    </row>
+    <row r="11" spans="2:15" ht="35.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="75" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="59"/>
+      <c r="H11" s="60">
+        <f>D5*24</f>
+        <v>96000</v>
+      </c>
+      <c r="I11" s="76"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="47"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="47"/>
+      <c r="O11" s="47"/>
+    </row>
+    <row r="12" spans="2:15" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C12" s="77" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="61">
+        <v>2000</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="59" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="59"/>
+      <c r="H12" s="60">
+        <v>125000</v>
+      </c>
+      <c r="I12" s="76"/>
+      <c r="K12" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="L12" s="48"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="48"/>
+      <c r="O12" s="48"/>
+    </row>
+    <row r="13" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C13" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="62">
+        <v>791</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="59" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="59"/>
+      <c r="H13" s="60">
+        <v>3000</v>
+      </c>
+      <c r="I13" s="76"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="48"/>
+      <c r="O13" s="48"/>
+    </row>
+    <row r="14" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C14" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="O6" s="79">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="19">
-        <v>0</v>
-      </c>
-      <c r="E7" s="64" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="65"/>
-      <c r="G7" s="70">
-        <f>G5-G6</f>
-        <v>1452</v>
-      </c>
-      <c r="H7" s="71"/>
-      <c r="I7" s="72"/>
-      <c r="N7" s="76" t="s">
-        <v>43</v>
-      </c>
-      <c r="O7" s="79">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="10">
-        <f>SUM(D5:D7)</f>
-        <v>7690</v>
-      </c>
-      <c r="I8" s="12"/>
-      <c r="N8" s="76" t="s">
-        <v>45</v>
-      </c>
-      <c r="O8" s="79">
-        <f>(D5+D6)*0.03</f>
-        <v>230.7</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="15"/>
-      <c r="D9" s="7"/>
-      <c r="I9" s="12"/>
-      <c r="N9" s="76" t="s">
-        <v>44</v>
-      </c>
-      <c r="O9" s="79">
-        <f>SUM(O5:O8)</f>
-        <v>2826.7</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" s="2" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B10" s="6"/>
-      <c r="C10" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="56"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="27"/>
-    </row>
-    <row r="11" spans="2:15" ht="35.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="75" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="75"/>
-      <c r="H11" s="36">
-        <f>D5*24</f>
-        <v>92280</v>
-      </c>
-      <c r="I11" s="21"/>
-    </row>
-    <row r="12" spans="2:15" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="8">
-        <v>2000</v>
-      </c>
-      <c r="E12" s="28"/>
-      <c r="F12" s="75" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" s="75"/>
-      <c r="H12" s="36">
-        <v>120000</v>
-      </c>
-      <c r="I12" s="21"/>
-    </row>
-    <row r="13" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="18">
-        <v>1000</v>
-      </c>
-      <c r="E13" s="28"/>
-      <c r="F13" s="75" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="75"/>
-      <c r="H13" s="36">
-        <v>3000</v>
-      </c>
-      <c r="I13" s="21"/>
-    </row>
-    <row r="14" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="18">
+      <c r="D14" s="62">
         <f>1150*2</f>
         <v>2300</v>
       </c>
-      <c r="E14" s="28"/>
-      <c r="F14" s="75" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" s="75"/>
-      <c r="H14" s="36">
-        <v>6000</v>
-      </c>
-      <c r="I14" s="21"/>
-    </row>
-    <row r="15" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="16" t="s">
+      <c r="E14" s="13"/>
+      <c r="F14" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="59"/>
+      <c r="H14" s="60">
+        <v>12000</v>
+      </c>
+      <c r="I14" s="76"/>
+      <c r="K14" s="48"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="48"/>
+      <c r="O14" s="48"/>
+    </row>
+    <row r="15" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C15" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="61">
         <v>50</v>
       </c>
-      <c r="E15" s="28"/>
-      <c r="F15" s="75" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="75"/>
-      <c r="H15" s="36">
+      <c r="E15" s="13"/>
+      <c r="F15" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="59"/>
+      <c r="H15" s="60">
         <v>3000</v>
       </c>
-      <c r="I15" s="21"/>
-    </row>
-    <row r="16" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="18">
+      <c r="I15" s="76"/>
+      <c r="K15" s="48"/>
+      <c r="L15" s="48"/>
+      <c r="M15" s="48"/>
+      <c r="N15" s="48"/>
+      <c r="O15" s="48"/>
+    </row>
+    <row r="16" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C16" s="77" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="62">
         <v>35</v>
       </c>
-      <c r="E16" s="28"/>
-      <c r="F16" s="75" t="s">
-        <v>27</v>
-      </c>
-      <c r="G16" s="75"/>
-      <c r="H16" s="36">
-        <v>6000</v>
-      </c>
-      <c r="I16" s="21"/>
-    </row>
-    <row r="17" spans="3:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="16" t="s">
+      <c r="E16" s="13"/>
+      <c r="F16" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="59"/>
+      <c r="H16" s="60">
+        <v>12000</v>
+      </c>
+      <c r="I16" s="76"/>
+      <c r="K16" s="48"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="48"/>
+      <c r="N16" s="48"/>
+      <c r="O16" s="48"/>
+    </row>
+    <row r="17" spans="3:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C17" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="61">
         <v>400</v>
       </c>
-      <c r="E17" s="28"/>
-      <c r="F17" s="75" t="s">
+      <c r="E17" s="13"/>
+      <c r="F17" s="59" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="59"/>
+      <c r="H17" s="60">
+        <f>SUM(H13:H16)</f>
+        <v>30000</v>
+      </c>
+      <c r="I17" s="76"/>
+    </row>
+    <row r="18" spans="3:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C18" s="77" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="62">
         <v>23</v>
       </c>
-      <c r="G17" s="75"/>
-      <c r="H17" s="36">
-        <f>SUM(H13:H16)</f>
-        <v>18000</v>
-      </c>
-      <c r="I17" s="21"/>
-    </row>
-    <row r="18" spans="3:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="16" t="s">
+      <c r="E18" s="13"/>
+      <c r="F18" s="59" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="59"/>
+      <c r="H18" s="60">
+        <f>H17*0.65</f>
+        <v>19500</v>
+      </c>
+      <c r="I18" s="76"/>
+    </row>
+    <row r="19" spans="3:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C19" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="18">
-        <v>23</v>
-      </c>
-      <c r="E18" s="28"/>
-      <c r="F18" s="75" t="s">
+      <c r="D19" s="62">
+        <v>70</v>
+      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" s="51"/>
+      <c r="H19" s="49">
+        <f>H12+H17</f>
+        <v>155000</v>
+      </c>
+      <c r="I19" s="76"/>
+    </row>
+    <row r="20" spans="3:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C20" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="G18" s="75"/>
-      <c r="H18" s="36">
-        <f>H17*0.65</f>
-        <v>11700</v>
-      </c>
-      <c r="I18" s="21"/>
-    </row>
-    <row r="19" spans="3:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="18">
-        <v>70</v>
-      </c>
-      <c r="E19" s="28"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="21"/>
-    </row>
-    <row r="20" spans="3:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="18">
+      <c r="D20" s="62">
         <v>50</v>
       </c>
-      <c r="E20" s="28"/>
-      <c r="F20" s="50" t="s">
+      <c r="E20" s="13"/>
+      <c r="F20" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="G20" s="51"/>
-      <c r="H20" s="37">
-        <f>H12+H17</f>
-        <v>138000</v>
-      </c>
-      <c r="I20" s="21"/>
-    </row>
-    <row r="21" spans="3:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="8">
+      <c r="G20" s="53"/>
+      <c r="H20" s="54">
+        <v>120000</v>
+      </c>
+      <c r="I20" s="76"/>
+    </row>
+    <row r="21" spans="3:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="77" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="61">
         <v>60</v>
       </c>
-      <c r="E21" s="28"/>
-      <c r="F21" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="G21" s="51"/>
-      <c r="H21" s="37">
-        <v>120000</v>
-      </c>
-      <c r="I21" s="21"/>
-    </row>
-    <row r="22" spans="3:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="31">
-        <v>250</v>
-      </c>
-      <c r="E22" s="28"/>
-      <c r="F22" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="G22" s="51"/>
-      <c r="H22" s="37">
+      <c r="E21" s="13"/>
+      <c r="F21" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" s="55"/>
+      <c r="H21" s="17">
         <f>H11+H18</f>
-        <v>103980</v>
-      </c>
-      <c r="I22" s="21"/>
-    </row>
-    <row r="23" spans="3:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C23" s="11" t="s">
+        <v>115500</v>
+      </c>
+      <c r="I21" s="76"/>
+    </row>
+    <row r="22" spans="3:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="24">
+      <c r="D22" s="79">
         <f>SUBTOTAL(109,Housing[Cost])</f>
-        <v>6238</v>
-      </c>
-      <c r="E23" s="29"/>
-      <c r="F23" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="G23" s="51"/>
-      <c r="H23" s="37">
+        <v>5779</v>
+      </c>
+      <c r="E22" s="80"/>
+      <c r="F22" s="81" t="s">
+        <v>36</v>
+      </c>
+      <c r="G22" s="82"/>
+      <c r="H22" s="83">
         <f>H11</f>
-        <v>92280</v>
-      </c>
-      <c r="I23" s="22"/>
-    </row>
-    <row r="24" spans="3:9" ht="24.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="3:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="3:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="3:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="3:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>96000</v>
+      </c>
+      <c r="I22" s="84"/>
+    </row>
+    <row r="23" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N6:O8">
     <sortCondition descending="1" ref="N5:N8"/>
   </sortState>
-  <mergeCells count="24">
+  <mergeCells count="26">
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="N4:O4"/>
@@ -2417,7 +2679,10 @@
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="K11:O11"/>
+    <mergeCell ref="K12:O16"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F22:G22"/>
     <mergeCell ref="C3:I3"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="E4:I4"/>
@@ -2431,7 +2696,6 @@
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F22:G22"/>
     <mergeCell ref="F11:G11"/>
   </mergeCells>
   <conditionalFormatting sqref="G7:I7">
@@ -2459,33 +2723,14 @@
     <ignoredError sqref="H17" formulaRange="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="27" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c6f9a84f66a9c8b9a21755b9ffafb945">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="27df39e3e7036dff54f89ddd5805ce72" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2791,7 +3036,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2800,26 +3045,27 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08AC7FD9-EBCF-4CC4-BE1C-34B80F7E8353}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A0798E9-19EF-47BB-B28E-84199D1A56C2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2840,10 +3086,29 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1766A65-F7C1-4A05-AEB7-FE8822B53FAC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08AC7FD9-EBCF-4CC4-BE1C-34B80F7E8353}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>